<commit_message>
small updates to data features notebook + GA runs
</commit_message>
<xml_diff>
--- a/results/wq/ga_calibration.xlsx
+++ b/results/wq/ga_calibration.xlsx
@@ -1063,28 +1063,28 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.5511691965937134</v>
+        <v>-0.936987634209313</v>
       </c>
       <c r="D11" t="n">
-        <v>0.005509734713870991</v>
+        <v>0.004373776166158113</v>
       </c>
       <c r="E11" t="n">
-        <v>0.008794623008401821</v>
+        <v>0.007749848631394511</v>
       </c>
       <c r="F11" t="n">
-        <v>2143.061055183411</v>
+        <v>2349.157398462296</v>
       </c>
       <c r="G11" t="n">
+        <v>-0.06064463945750895</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-0.1451544681756371</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.07491938837368262</v>
+      </c>
+      <c r="J11" t="n">
         <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>-0.2333835605476369</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>-0.04653909717644134</v>
       </c>
     </row>
     <row r="12">

</xml_diff>

<commit_message>
updated water quality data
</commit_message>
<xml_diff>
--- a/results/wq/ga_calibration.xlsx
+++ b/results/wq/ga_calibration.xlsx
@@ -1223,15 +1223,35 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>wwmd</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.6625668846702162</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.001545301883302395</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0009759820188660768</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10724.66072463989</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-0.02545172565787205</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-0.03511352692945889</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.07780546049260043</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">

</xml_diff>

<commit_message>
modified design of experiments function for training gaussian process model
</commit_message>
<xml_diff>
--- a/results/wq/ga_calibration.xlsx
+++ b/results/wq/ga_calibration.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="500" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="single" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="material-only" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="material-age-diameter" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="material-age-mrt" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="material-age-velocity" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Aptos Narrow"/>
       <charset val="1"/>
@@ -48,6 +48,11 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -59,12 +64,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -92,23 +112,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -375,11 +394,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col width="17.265625" customWidth="1" style="3" min="1" max="1"/>
-    <col width="11.73046875" customWidth="1" style="3" min="2" max="6"/>
+    <col width="17.265625" customWidth="1" min="1" max="1"/>
+    <col width="11.73046875" customWidth="1" min="2" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>worksheet</t>
@@ -411,7 +430,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>single</t>
@@ -423,7 +442,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>material-only</t>
@@ -440,7 +459,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="3">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
           <t>material-age-diameter</t>
@@ -472,7 +491,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="3">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>material-age-mrt</t>
@@ -518,81 +537,81 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col width="8.59765625" customWidth="1" style="3" min="1" max="1"/>
-    <col width="18.265625" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
-    <col width="18.265625" customWidth="1" style="3" min="3" max="3"/>
-    <col width="9.86328125" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="8.59765625" customWidth="1" style="3" min="5" max="16384"/>
+    <col width="8.59765625" customWidth="1" min="1" max="1"/>
+    <col width="18.265625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="18.265625" customWidth="1" min="3" max="3"/>
+    <col width="9.86328125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8.59765625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>data_period</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>demand_resolution</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>wq_sensors_used</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>bulk_coeff</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>train_mse</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>test_mse</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>cpu_time</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>G0</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3"/>
-    <row r="3" ht="15" customHeight="1" s="3"/>
-    <row r="4" ht="15" customHeight="1" s="3"/>
-    <row r="5" ht="15" customHeight="1" s="3"/>
-    <row r="6" ht="15" customHeight="1" s="3"/>
-    <row r="7" ht="15" customHeight="1" s="3"/>
-    <row r="8" ht="15" customHeight="1" s="3"/>
-    <row r="9" ht="15" customHeight="1" s="3"/>
-    <row r="10" ht="15" customHeight="1" s="3"/>
-    <row r="11" ht="15" customHeight="1" s="3"/>
-    <row r="12" ht="15" customHeight="1" s="3"/>
-    <row r="13" ht="15" customHeight="1" s="3"/>
-    <row r="14" ht="15" customHeight="1" s="3"/>
-    <row r="15" ht="15" customHeight="1" s="3"/>
-    <row r="16" ht="15" customHeight="1" s="3"/>
-    <row r="17" ht="15" customHeight="1" s="3"/>
-    <row r="18" ht="15" customHeight="1" s="3"/>
-    <row r="19" ht="15" customHeight="1" s="3"/>
-    <row r="20" ht="15" customHeight="1" s="3"/>
-    <row r="21" ht="15" customHeight="1" s="3"/>
+    <row r="2" ht="15" customHeight="1"/>
+    <row r="3" ht="15" customHeight="1"/>
+    <row r="4" ht="15" customHeight="1"/>
+    <row r="5" ht="15" customHeight="1"/>
+    <row r="6" ht="15" customHeight="1"/>
+    <row r="7" ht="15" customHeight="1"/>
+    <row r="8" ht="15" customHeight="1"/>
+    <row r="9" ht="15" customHeight="1"/>
+    <row r="10" ht="15" customHeight="1"/>
+    <row r="11" ht="15" customHeight="1"/>
+    <row r="12" ht="15" customHeight="1"/>
+    <row r="13" ht="15" customHeight="1"/>
+    <row r="14" ht="15" customHeight="1"/>
+    <row r="15" ht="15" customHeight="1"/>
+    <row r="16" ht="15" customHeight="1"/>
+    <row r="17" ht="15" customHeight="1"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="19" ht="15" customHeight="1"/>
+    <row r="20" ht="15" customHeight="1"/>
+    <row r="21" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -613,82 +632,82 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col width="11.86328125" customWidth="1" style="3" min="1" max="1"/>
-    <col width="18.3984375" customWidth="1" style="3" min="2" max="3"/>
-    <col width="12.86328125" customWidth="1" style="3" min="4" max="4"/>
-    <col width="10.53125" customWidth="1" style="3" min="5" max="5"/>
-    <col width="8.59765625" customWidth="1" style="3" min="6" max="7"/>
-    <col width="13.53125" customWidth="1" style="3" min="8" max="9"/>
-    <col width="8.59765625" customWidth="1" style="3" min="10" max="16384"/>
+    <col width="11.86328125" customWidth="1" min="1" max="1"/>
+    <col width="18.3984375" customWidth="1" min="2" max="3"/>
+    <col width="12.86328125" customWidth="1" min="4" max="4"/>
+    <col width="10.53125" customWidth="1" min="5" max="5"/>
+    <col width="8.59765625" customWidth="1" min="6" max="7"/>
+    <col width="13.53125" customWidth="1" min="8" max="9"/>
+    <col width="8.59765625" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>data_period</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>demand_resolution</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>wq_sensors_used</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>bulk_coeff</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>train_mse</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>test_mse</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>cpu_time</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>G0</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>G1</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3"/>
-    <row r="3" ht="15" customHeight="1" s="3"/>
-    <row r="4" ht="15" customHeight="1" s="3"/>
-    <row r="5" ht="15" customHeight="1" s="3"/>
-    <row r="6" ht="15" customHeight="1" s="3"/>
-    <row r="7" ht="15" customHeight="1" s="3"/>
-    <row r="8" ht="15" customHeight="1" s="3"/>
-    <row r="9" ht="15" customHeight="1" s="3"/>
-    <row r="10" ht="15" customHeight="1" s="3"/>
-    <row r="11" ht="15" customHeight="1" s="3"/>
-    <row r="12" ht="15" customHeight="1" s="3"/>
-    <row r="13" ht="15" customHeight="1" s="3"/>
-    <row r="14" ht="15" customHeight="1" s="3"/>
-    <row r="15" ht="15" customHeight="1" s="3"/>
-    <row r="16" ht="15" customHeight="1" s="3"/>
-    <row r="17" ht="15" customHeight="1" s="3"/>
-    <row r="18" ht="15" customHeight="1" s="3"/>
-    <row r="19" ht="15" customHeight="1" s="3"/>
-    <row r="20" ht="15" customHeight="1" s="3"/>
-    <row r="21" ht="15" customHeight="1" s="3"/>
+    <row r="2" ht="15" customHeight="1"/>
+    <row r="3" ht="15" customHeight="1"/>
+    <row r="4" ht="15" customHeight="1"/>
+    <row r="5" ht="15" customHeight="1"/>
+    <row r="6" ht="15" customHeight="1"/>
+    <row r="7" ht="15" customHeight="1"/>
+    <row r="8" ht="15" customHeight="1"/>
+    <row r="9" ht="15" customHeight="1"/>
+    <row r="10" ht="15" customHeight="1"/>
+    <row r="11" ht="15" customHeight="1"/>
+    <row r="12" ht="15" customHeight="1"/>
+    <row r="13" ht="15" customHeight="1"/>
+    <row r="14" ht="15" customHeight="1"/>
+    <row r="15" ht="15" customHeight="1"/>
+    <row r="16" ht="15" customHeight="1"/>
+    <row r="17" ht="15" customHeight="1"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="19" ht="15" customHeight="1"/>
+    <row r="20" ht="15" customHeight="1"/>
+    <row r="21" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -701,7 +720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -710,62 +729,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>data_period</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>demand_resolution</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>wq_sensors_used</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>bulk_coeff</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>train_mse</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>test_mse</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>cpu_time</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>G0</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="6" t="inlineStr">
         <is>
           <t>G1</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="6" t="inlineStr">
         <is>
           <t>G2</t>
         </is>
       </c>
-      <c r="K1" s="7" t="inlineStr">
+      <c r="K1" s="6" t="inlineStr">
         <is>
           <t>G3</t>
         </is>
       </c>
-      <c r="L1" s="7" t="inlineStr">
+      <c r="L1" s="6" t="inlineStr">
         <is>
           <t>G4</t>
         </is>
@@ -811,6 +830,90 @@
       </c>
       <c r="L2" t="n">
         <v>-0.01</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wwmd</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>kiosk only</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.5126061925831822</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.001122609200955326</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001275515361691412</v>
+      </c>
+      <c r="G3" t="n">
+        <v>15433.73804163933</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-0.1937379419510491</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.1072255400286369</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-0.03883206613208263</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1.929727004422416e-05</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.04997695755738575</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>20</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wwmd</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>kiosk only</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.5126061925831822</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.001122609200955326</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001275515361691412</v>
+      </c>
+      <c r="G4" t="n">
+        <v>15433.73804163933</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.1937379419510491</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.1072255400286369</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.03883206613208263</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1.929727004422416e-05</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.04997695755738575</v>
       </c>
     </row>
   </sheetData>
@@ -826,77 +929,78 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="9.06640625" customWidth="1" style="6" min="1" max="1"/>
-    <col width="12.1328125" customWidth="1" style="6" min="2" max="3"/>
-    <col width="11.06640625" customWidth="1" style="6" min="4" max="4"/>
-    <col width="9.06640625" customWidth="1" style="6" min="5" max="7"/>
-    <col width="12.3984375" customWidth="1" style="6" min="8" max="8"/>
-    <col width="9.06640625" customWidth="1" style="6" min="9" max="16384"/>
+    <col width="9.06640625" customWidth="1" style="4" min="1" max="1"/>
+    <col width="12.1328125" customWidth="1" style="4" min="2" max="3"/>
+    <col width="11.06640625" customWidth="1" style="4" min="4" max="4"/>
+    <col width="9.06640625" customWidth="1" style="4" min="5" max="7"/>
+    <col width="12.3984375" customWidth="1" style="4" min="8" max="8"/>
+    <col width="9.06640625" customWidth="1" style="4" min="9" max="9"/>
+    <col width="9.06640625" customWidth="1" style="4" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>data_period</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>demand_resolution</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>wq_sensors_used</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>bulk_coeff</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>train_mse</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>test_mse</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>cpu_time</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>G0</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>G1</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>G2</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>G3</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>G4</t>
         </is>

</xml_diff>

<commit_message>
updated mcmc notebook using pymc package; to tidy and move functions to src at later date
</commit_message>
<xml_diff>
--- a/results/wq/ga_calibration.xlsx
+++ b/results/wq/ga_calibration.xlsx
@@ -824,7 +824,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1020,6 +1020,132 @@
         <v>-0.2</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>wwmd</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>kiosk + hydrant</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.7966854185018963</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.006704448355048949</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.008156122999893109</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5358.539281606674</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-0.0145914976373844</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-0.1960026948329951</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-0.1480531118982936</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-0.06934176270382052</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-0.01000927001696754</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>wwmd</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kiosk + hydrant</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.6625668846702162</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.00154224852862009</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0009395606420866699</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7634.565146446228</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.01029578055671602</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.02213087515193186</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.3651462109107909</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.03409693106586862</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.1276630981074167</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>16</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>wwmd</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kiosk + hydrant</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.6572141270400695</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0105418661906856</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.007352559039659772</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16508.92272257805</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.01000529444249022</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.01844996715188763</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-0.04490408910009593</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-0.09613977806487756</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.01000286903281968</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>